<commit_message>
Do a Lerp test
</commit_message>
<xml_diff>
--- a/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
+++ b/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>Friday</t>
   </si>
@@ -41,10 +41,28 @@
     <t>Thursday</t>
   </si>
   <si>
-    <t>Study GnG enemy behavior</t>
-  </si>
-  <si>
     <t>Pseudocode out what to do</t>
+  </si>
+  <si>
+    <t>Review Transform Manipulation</t>
+  </si>
+  <si>
+    <t>Review Component Access</t>
+  </si>
+  <si>
+    <t>Make Plan for the rest of the week</t>
+  </si>
+  <si>
+    <t>Take notes on enemies</t>
+  </si>
+  <si>
+    <t>Pseudocode out Zombie behavior</t>
+  </si>
+  <si>
+    <t>Past</t>
+  </si>
+  <si>
+    <t>Study GnG enemy (zombie) behavior</t>
   </si>
 </sst>
 </file>
@@ -60,12 +78,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -80,8 +104,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,17 +390,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K3"/>
+  <dimension ref="B1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" customWidth="1"/>
     <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="14" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" customWidth="1"/>
+    <col min="5" max="14" width="21.85546875" customWidth="1"/>
     <col min="15" max="15" width="63.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -410,12 +440,36 @@
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Got a GameObject moving horizontally
</commit_message>
<xml_diff>
--- a/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
+++ b/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>Friday</t>
   </si>
@@ -56,13 +56,25 @@
     <t>Take notes on enemies</t>
   </si>
   <si>
-    <t>Pseudocode out Zombie behavior</t>
-  </si>
-  <si>
     <t>Past</t>
   </si>
   <si>
     <t>Study GnG enemy (zombie) behavior</t>
+  </si>
+  <si>
+    <t>Get an object moving</t>
+  </si>
+  <si>
+    <t>Pseudocode out Zombie movement behavior</t>
+  </si>
+  <si>
+    <t>Download a Zombie Sprite</t>
+  </si>
+  <si>
+    <t>Figure out how to change direction</t>
+  </si>
+  <si>
+    <t>Attempt a lerp zombie movement implementation</t>
   </si>
 </sst>
 </file>
@@ -104,12 +116,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,7 +409,7 @@
   <dimension ref="B1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -402,7 +418,8 @@
     <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.85546875" customWidth="1"/>
-    <col min="5" max="14" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="14" width="21.85546875" customWidth="1"/>
     <col min="15" max="15" width="63.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -440,31 +457,44 @@
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>8</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C5" s="2" t="s">
-        <v>12</v>
+    <row r="5" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Managed to make a variable endpoint
</commit_message>
<xml_diff>
--- a/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
+++ b/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Friday</t>
   </si>
@@ -75,6 +75,18 @@
   </si>
   <si>
     <t>Attempt a lerp zombie movement implementation</t>
+  </si>
+  <si>
+    <t>Pseudocode Zombie Spawn</t>
+  </si>
+  <si>
+    <t>Pseudocode Zombie Spawner Behavior</t>
+  </si>
+  <si>
+    <t>Implement Sprite and figure out how to reverse zombie movement in spawner</t>
+  </si>
+  <si>
+    <t>Make target a variable off camera</t>
   </si>
 </sst>
 </file>
@@ -116,8 +128,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -126,6 +141,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K6"/>
+  <dimension ref="B1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,11 +437,11 @@
     <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.85546875" customWidth="1"/>
     <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="14" width="21.85546875" customWidth="1"/>
-    <col min="15" max="15" width="63.7109375" customWidth="1"/>
+    <col min="6" max="15" width="21.85546875" customWidth="1"/>
+    <col min="16" max="16" width="63.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -440,66 +458,80 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="5" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="C5" s="1" t="s">
+    <row r="5" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="E5" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" ht="60" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sliced the photos and added a Zombie Spawner
</commit_message>
<xml_diff>
--- a/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
+++ b/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>Friday</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Make a zombie destantiator</t>
+  </si>
+  <si>
+    <t>If done, make plan for Thursday</t>
   </si>
 </sst>
 </file>
@@ -131,7 +134,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -140,12 +143,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -427,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L7"/>
+  <dimension ref="B1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,18 +491,18 @@
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -511,7 +513,7 @@
       <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -522,7 +524,7 @@
       <c r="D5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -540,6 +542,11 @@
     <row r="7" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="E7" s="1" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="E8" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented some random zombie spawning
</commit_message>
<xml_diff>
--- a/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
+++ b/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
@@ -89,9 +89,6 @@
     <t>Make a zombie destantiator</t>
   </si>
   <si>
-    <t>If done, make plan for Friday</t>
-  </si>
-  <si>
     <t>Make randomized but player relative spawning locations</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>Implement Sprite</t>
+  </si>
+  <si>
+    <t>If done, make plan for Saturday</t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,7 @@
   <dimension ref="B1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,7 +500,7 @@
       <c r="E2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -512,10 +512,10 @@
         <v>13</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="30" x14ac:dyDescent="0.25">
@@ -528,7 +528,7 @@
       <c r="E4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -542,8 +542,8 @@
       <c r="E5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>21</v>
+      <c r="G5" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="45" x14ac:dyDescent="0.25">
@@ -553,8 +553,8 @@
       <c r="D6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>22</v>
+      <c r="G6" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Got camera relative despawns. There's also a blank zombie direction script rn.
</commit_message>
<xml_diff>
--- a/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
+++ b/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
@@ -98,7 +98,7 @@
     <t>Implement Sprite</t>
   </si>
   <si>
-    <t>If done, make plan for Saturday</t>
+    <t>If done, make plan for Monday</t>
   </si>
 </sst>
 </file>
@@ -528,7 +528,7 @@
       <c r="E4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="3" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Failed attempts to make left-moving zombie
</commit_message>
<xml_diff>
--- a/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
+++ b/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
@@ -98,7 +98,7 @@
     <t>Implement Sprite</t>
   </si>
   <si>
-    <t>If done, make plan for Monday</t>
+    <t>If done, make plan for Tuesday</t>
   </si>
 </sst>
 </file>
@@ -437,8 +437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,7 +500,7 @@
       <c r="E2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -514,7 +514,7 @@
       <c r="E3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -542,7 +542,7 @@
       <c r="E5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -553,7 +553,7 @@
       <c r="D6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="3" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implemented reflected zombie image
</commit_message>
<xml_diff>
--- a/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
+++ b/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>Friday</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>If done, make plan for Tuesday</t>
+  </si>
+  <si>
+    <t>Flip Zombie Image</t>
   </si>
 </sst>
 </file>
@@ -435,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L6"/>
+  <dimension ref="B1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,6 +560,11 @@
         <v>21</v>
       </c>
     </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H7" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Figure out mirrored images
</commit_message>
<xml_diff>
--- a/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
+++ b/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
@@ -98,10 +98,10 @@
     <t>Implement Sprite</t>
   </si>
   <si>
-    <t>If done, make plan for Tuesday</t>
-  </si>
-  <si>
     <t>Flip Zombie Image</t>
+  </si>
+  <si>
+    <t>If done, make plan for Wednesday</t>
   </si>
 </sst>
 </file>
@@ -440,8 +440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,7 +503,7 @@
       <c r="E2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -517,7 +517,7 @@
       <c r="E3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -545,8 +545,8 @@
       <c r="E5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>24</v>
+      <c r="I5" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="45" x14ac:dyDescent="0.25">
@@ -562,7 +562,7 @@
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I finished the zombie and started adding audio
</commit_message>
<xml_diff>
--- a/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
+++ b/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>Friday</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>If done, make plan for Wednesday</t>
+  </si>
+  <si>
+    <t>Start work on Zombie Animation</t>
+  </si>
+  <si>
+    <t>Make camera position dependent on player</t>
   </si>
 </sst>
 </file>
@@ -143,16 +149,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -441,7 +444,7 @@
   <dimension ref="B1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,7 +454,9 @@
     <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.85546875" customWidth="1"/>
     <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="15" width="21.85546875" customWidth="1"/>
+    <col min="6" max="8" width="21.85546875" customWidth="1"/>
+    <col min="9" max="9" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="15" width="21.85546875" customWidth="1"/>
     <col min="16" max="16" width="63.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -500,10 +505,10 @@
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -517,7 +522,7 @@
       <c r="E3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -534,6 +539,9 @@
       <c r="G4" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="I4" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="5" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
@@ -558,6 +566,9 @@
       </c>
       <c r="G6" s="3" t="s">
         <v>21</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Start scene to test Arthur out
</commit_message>
<xml_diff>
--- a/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
+++ b/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>Friday</t>
   </si>
@@ -108,6 +108,18 @@
   </si>
   <si>
     <t>Make camera position dependent on player</t>
+  </si>
+  <si>
+    <t>Add song to scene</t>
+  </si>
+  <si>
+    <t>Pseudocode out Arthur Jump</t>
+  </si>
+  <si>
+    <t>Implement Arthur Jump</t>
+  </si>
+  <si>
+    <t>Implement Arthur Sprite</t>
   </si>
 </sst>
 </file>
@@ -444,7 +456,7 @@
   <dimension ref="B1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,7 +468,8 @@
     <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="21.85546875" customWidth="1"/>
     <col min="9" max="9" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="15" width="21.85546875" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" customWidth="1"/>
+    <col min="11" max="15" width="21.85546875" customWidth="1"/>
     <col min="16" max="16" width="63.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -511,6 +524,9 @@
       <c r="I2" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="J2" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="3" spans="2:12" ht="60" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
@@ -525,6 +541,9 @@
       <c r="I3" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="J3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="4" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
@@ -542,6 +561,9 @@
       <c r="I4" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="J4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="5" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
@@ -553,7 +575,7 @@
       <c r="E5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="3" t="s">
         <v>25</v>
       </c>
     </row>
@@ -567,13 +589,16 @@
       <c r="G6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H7" s="3" t="s">
         <v>24</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Start Arthur Player Controller
</commit_message>
<xml_diff>
--- a/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
+++ b/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>Friday</t>
   </si>
@@ -125,7 +125,10 @@
     <t>Experiment with randomizing zombie velocities</t>
   </si>
   <si>
-    <t>Make Plan For Thursday</t>
+    <t>Pick between physics and direct transform</t>
+  </si>
+  <si>
+    <t>Make Plan For Friday</t>
   </si>
 </sst>
 </file>
@@ -462,7 +465,7 @@
   <dimension ref="B1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,11 +533,11 @@
       <c r="I2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" ht="45" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
@@ -547,7 +550,7 @@
       <c r="I3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>30</v>
       </c>
     </row>
@@ -567,7 +570,7 @@
       <c r="I4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>31</v>
       </c>
     </row>
@@ -587,6 +590,9 @@
       <c r="J5" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="K5" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="6" spans="2:12" ht="45" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
@@ -601,8 +607,8 @@
       <c r="I6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J6" t="s">
-        <v>33</v>
+      <c r="K6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Switched Arthur Jump to Physics based calculations
</commit_message>
<xml_diff>
--- a/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
+++ b/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
@@ -465,7 +465,7 @@
   <dimension ref="B1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,7 +533,7 @@
       <c r="I2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -550,7 +550,7 @@
       <c r="I3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>30</v>
       </c>
     </row>
@@ -590,7 +590,7 @@
       <c r="J5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" s="3" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Introduce a simple raycast based groundcheck
</commit_message>
<xml_diff>
--- a/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
+++ b/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
   <si>
     <t>Friday</t>
   </si>
@@ -129,6 +130,15 @@
   </si>
   <si>
     <t>Make Plan For Friday</t>
+  </si>
+  <si>
+    <t>Implement a raycast based groundcheck</t>
+  </si>
+  <si>
+    <t>Start designing levels</t>
+  </si>
+  <si>
+    <t>Credit Controller Code creators</t>
   </si>
 </sst>
 </file>
@@ -170,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -180,6 +190,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -464,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,4 +635,80 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:K4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" customWidth="1"/>
+    <col min="8" max="8" width="27.85546875" customWidth="1"/>
+    <col min="9" max="9" width="28.5703125" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" customWidth="1"/>
+    <col min="11" max="11" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finish raycast check and make plan for next two days
</commit_message>
<xml_diff>
--- a/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
+++ b/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
   <si>
     <t>Friday</t>
   </si>
@@ -138,7 +138,28 @@
     <t>Start designing levels</t>
   </si>
   <si>
-    <t>Credit Controller Code creators</t>
+    <t>Implement boxcast based groundcheck</t>
+  </si>
+  <si>
+    <t>Credit Controller Code authors I ripped off</t>
+  </si>
+  <si>
+    <t>Research guidelines for making good levels and level ideas</t>
+  </si>
+  <si>
+    <t>Figure out timeline for efficient level workflow dev</t>
+  </si>
+  <si>
+    <t>Pseudocode out what I need for the levels</t>
+  </si>
+  <si>
+    <t>Program Easiest Level</t>
+  </si>
+  <si>
+    <t>Maybe program objects to be used in later levels</t>
+  </si>
+  <si>
+    <t>Plan for Friday and next week</t>
   </si>
 </sst>
 </file>
@@ -180,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -195,6 +216,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -639,16 +661,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K4"/>
+  <dimension ref="B1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="54.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.28515625" customWidth="1"/>
     <col min="6" max="6" width="20.85546875" customWidth="1"/>
     <col min="7" max="7" width="25.140625" customWidth="1"/>
@@ -694,18 +716,56 @@
       <c r="B2" t="s">
         <v>35</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>36</v>
       </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
         <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement boxcast based groundcheck
</commit_message>
<xml_diff>
--- a/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
+++ b/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
@@ -664,7 +664,7 @@
   <dimension ref="B1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,7 +746,7 @@
       <c r="C5" t="s">
         <v>37</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Resume Progress. Change effector and player tag properties
</commit_message>
<xml_diff>
--- a/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
+++ b/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
@@ -16,6 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="52">
   <si>
     <t>Friday</t>
   </si>
@@ -163,6 +164,24 @@
   </si>
   <si>
     <t>Plan for next week</t>
+  </si>
+  <si>
+    <t>Plan for this week is levels</t>
+  </si>
+  <si>
+    <t>Two main mechanics id'd: Jumping and block pushing</t>
+  </si>
+  <si>
+    <t>Write some level "stories" similar to what Maddy Thorsen was talking about</t>
+  </si>
+  <si>
+    <t>Brainstorm Ideas</t>
+  </si>
+  <si>
+    <t>Maybe attempt Thorsen's story exercise on levels from platformers you like?</t>
+  </si>
+  <si>
+    <t>Watch Mark Brown's level design videos?</t>
   </si>
 </sst>
 </file>
@@ -666,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,7 +694,7 @@
     <col min="2" max="2" width="37.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="54.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.85546875" customWidth="1"/>
+    <col min="8" max="8" width="69.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28.5703125" customWidth="1"/>
     <col min="10" max="10" width="20.28515625" customWidth="1"/>
     <col min="11" max="11" width="20" customWidth="1"/>
@@ -723,6 +742,15 @@
       <c r="E2" t="s">
         <v>42</v>
       </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
@@ -734,6 +762,9 @@
       <c r="E3" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="H3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
@@ -748,6 +779,9 @@
       <c r="G4" t="s">
         <v>45</v>
       </c>
+      <c r="H4" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
@@ -756,6 +790,9 @@
       <c r="D5" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="H5" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C6" s="6" t="s">
@@ -767,15 +804,24 @@
       <c r="E6" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="H6" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>40</v>
       </c>
+      <c r="H7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>41</v>
+      </c>
+      <c r="H8" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make a new scene
</commit_message>
<xml_diff>
--- a/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
+++ b/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
@@ -16,7 +16,6 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="53">
   <si>
     <t>Friday</t>
   </si>
@@ -182,6 +181,9 @@
   </si>
   <si>
     <t>Watch Mark Brown's level design videos?</t>
+  </si>
+  <si>
+    <t>Fix Groundcheck issues in player controller that causes groundcheck to sometimes fail groundcheck</t>
   </si>
 </sst>
 </file>
@@ -683,10 +685,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K8"/>
+  <dimension ref="B1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,7 +697,7 @@
     <col min="3" max="5" width="54.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="69.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.5703125" customWidth="1"/>
+    <col min="9" max="9" width="91" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.28515625" customWidth="1"/>
     <col min="11" max="11" width="20" customWidth="1"/>
   </cols>
@@ -751,6 +753,9 @@
       <c r="H2" t="s">
         <v>42</v>
       </c>
+      <c r="I2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
@@ -765,6 +770,9 @@
       <c r="H3" t="s">
         <v>48</v>
       </c>
+      <c r="I3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
@@ -782,6 +790,9 @@
       <c r="H4" t="s">
         <v>49</v>
       </c>
+      <c r="I4" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
@@ -793,6 +804,9 @@
       <c r="H5" t="s">
         <v>46</v>
       </c>
+      <c r="I5" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C6" s="6" t="s">
@@ -815,6 +829,9 @@
       <c r="H7" t="s">
         <v>50</v>
       </c>
+      <c r="I7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
@@ -822,6 +839,14 @@
       </c>
       <c r="H8" t="s">
         <v>51</v>
+      </c>
+      <c r="I8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make new scenes and update plans
</commit_message>
<xml_diff>
--- a/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
+++ b/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
@@ -694,7 +694,7 @@
   <dimension ref="B1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,7 +776,7 @@
       <c r="H3" t="s">
         <v>48</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="2" t="s">
         <v>48</v>
       </c>
     </row>
@@ -851,7 +851,7 @@
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I9" t="s">
+      <c r="I9" s="2" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finish up for today
</commit_message>
<xml_diff>
--- a/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
+++ b/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="58">
   <si>
     <t>Friday</t>
   </si>
@@ -189,7 +189,16 @@
     <t>Make sure pre-fabs are tagged correctly</t>
   </si>
   <si>
-    <t>Implement BlockPulling with a key</t>
+    <t>Attempt Thorsen's story exercise on a Bubsy 3D level just for fun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement Jeremy's Movement Script Modifications </t>
+  </si>
+  <si>
+    <t>Implement BlockPulling script with a key</t>
+  </si>
+  <si>
+    <t>Unimplement the mods</t>
   </si>
 </sst>
 </file>
@@ -691,10 +700,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K11"/>
+  <dimension ref="B1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,7 +713,7 @@
     <col min="6" max="7" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="69.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="91" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.28515625" customWidth="1"/>
+    <col min="10" max="10" width="70.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20" customWidth="1"/>
   </cols>
   <sheetData>
@@ -762,6 +771,9 @@
       <c r="I2" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="J2" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
@@ -779,6 +791,9 @@
       <c r="I3" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="J3" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
@@ -796,7 +811,7 @@
       <c r="H4" t="s">
         <v>49</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="2" t="s">
         <v>49</v>
       </c>
     </row>
@@ -838,6 +853,9 @@
       <c r="I7" t="s">
         <v>50</v>
       </c>
+      <c r="J7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
@@ -859,9 +877,23 @@
       <c r="I10" t="s">
         <v>53</v>
       </c>
+      <c r="J10" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="I11" t="s">
+        <v>56</v>
+      </c>
+      <c r="J11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>54</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Make a new scene and make plan for today
</commit_message>
<xml_diff>
--- a/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
+++ b/PersonalProj/GhostsGoblinsEnemiesPlan.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="59">
   <si>
     <t>Friday</t>
   </si>
@@ -199,6 +199,9 @@
   </si>
   <si>
     <t>Unimplement the mods</t>
+  </si>
+  <si>
+    <t>Stop wall sticking behavior</t>
   </si>
 </sst>
 </file>
@@ -703,7 +706,7 @@
   <dimension ref="B1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,7 +717,7 @@
     <col min="8" max="8" width="69.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="91" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="70.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20" customWidth="1"/>
+    <col min="11" max="11" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
@@ -814,6 +817,9 @@
       <c r="I4" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="K4" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
@@ -877,7 +883,7 @@
       <c r="I10" t="s">
         <v>53</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="2" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>